<commit_message>
Fixed trap deployment time issues in a few data files. Updated readPhytos.R with new data. Wrote code to calulate trap deployment duration and retrieval/deployment times.i
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/CIN/CH4_157_Storrie/dataSheets/surgeData157.xlsx
+++ b/SuRGE_Sharepoint/data/CIN/CH4_157_Storrie/dataSheets/surgeData157.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/CIN/CH4_157_Storrie/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1512" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8130F79-AF13-467E-8D59-245CE683D8AA}"/>
+  <xr:revisionPtr revIDLastSave="1513" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E996CC9D-80EB-4A4B-B64A-103BB8AD13F3}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="34560" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4830" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1359,6 +1359,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1659,8 +1663,8 @@
   <dimension ref="A1:BZ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BX4" sqref="BX4"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G3" sqref="G3:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,7 +2081,7 @@
         <v>190</v>
       </c>
       <c r="G3" s="26">
-        <v>0.23055555555555554</v>
+        <v>0.73055555555555562</v>
       </c>
       <c r="H3" t="s">
         <v>191</v>
@@ -2187,7 +2191,7 @@
         <v>190</v>
       </c>
       <c r="G4" s="26">
-        <v>0.2388888888888889</v>
+        <v>0.73888888888888893</v>
       </c>
       <c r="H4" t="s">
         <v>191</v>
@@ -2297,7 +2301,7 @@
         <v>190</v>
       </c>
       <c r="G5" s="26">
-        <v>0.32777777777777778</v>
+        <v>0.82777777777777783</v>
       </c>
       <c r="H5" t="s">
         <v>191</v>
@@ -2395,7 +2399,7 @@
         <v>190</v>
       </c>
       <c r="G6" s="26">
-        <v>0.22569444444444445</v>
+        <v>0.72569444444444453</v>
       </c>
       <c r="H6" t="s">
         <v>191</v>
@@ -2493,7 +2497,7 @@
         <v>190</v>
       </c>
       <c r="G7" s="26">
-        <v>0.25555555555555559</v>
+        <v>0.75555555555555554</v>
       </c>
       <c r="H7" t="s">
         <v>191</v>
@@ -2591,7 +2595,7 @@
         <v>190</v>
       </c>
       <c r="G8" s="26">
-        <v>0.26041666666666669</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="H8" t="s">
         <v>191</v>
@@ -2689,7 +2693,7 @@
         <v>190</v>
       </c>
       <c r="G9" s="26">
-        <v>0.27777777777777779</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="H9" t="s">
         <v>191</v>
@@ -2787,7 +2791,7 @@
         <v>190</v>
       </c>
       <c r="G10" s="26">
-        <v>0.26874999999999999</v>
+        <v>0.76874999999999993</v>
       </c>
       <c r="H10" t="s">
         <v>191</v>
@@ -2861,7 +2865,7 @@
         <v>190</v>
       </c>
       <c r="G11" s="26">
-        <v>0.27430555555555552</v>
+        <v>0.77430555555555547</v>
       </c>
       <c r="H11" t="s">
         <v>191</v>
@@ -2959,7 +2963,7 @@
         <v>190</v>
       </c>
       <c r="G12" s="26">
-        <v>0.30277777777777776</v>
+        <v>0.8027777777777777</v>
       </c>
       <c r="H12" t="s">
         <v>191</v>
@@ -3057,7 +3061,7 @@
         <v>190</v>
       </c>
       <c r="G13" s="26">
-        <v>0.29930555555555555</v>
+        <v>0.7993055555555556</v>
       </c>
       <c r="H13" t="s">
         <v>191</v>
@@ -3155,7 +3159,7 @@
         <v>190</v>
       </c>
       <c r="G14" s="26">
-        <v>0.29652777777777778</v>
+        <v>0.79652777777777783</v>
       </c>
       <c r="H14" t="s">
         <v>191</v>
@@ -3253,7 +3257,7 @@
         <v>190</v>
       </c>
       <c r="G15" s="26">
-        <v>0.31388888888888888</v>
+        <v>0.81388888888888899</v>
       </c>
       <c r="H15" t="s">
         <v>191</v>
@@ -3327,7 +3331,7 @@
         <v>190</v>
       </c>
       <c r="G16" s="26">
-        <v>0.3215277777777778</v>
+        <v>0.82152777777777775</v>
       </c>
       <c r="H16" t="s">
         <v>191</v>
@@ -3425,7 +3429,7 @@
         <v>190</v>
       </c>
       <c r="G17" s="26">
-        <v>0.31041666666666667</v>
+        <v>0.81041666666666667</v>
       </c>
       <c r="H17" t="s">
         <v>191</v>
@@ -5183,20 +5187,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
@@ -5238,6 +5228,20 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F113896-8C4C-43AA-B27A-761A581C3BEE}">
   <ds:schemaRefs>
@@ -5262,9 +5266,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5278,15 +5288,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>